<commit_message>
Fixed usages list for cp format
</commit_message>
<xml_diff>
--- a/core/import_data/resources/usages_cp_format.xlsx
+++ b/core/import_data/resources/usages_cp_format.xlsx
@@ -7,11 +7,16 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="OddBsQhMkWxwp9ho2KCyOfeMNqk6lCsovT/OT303tz8="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>usage</t>
   </si>
@@ -61,7 +66,10 @@
     <t>Refrigeration Servicing</t>
   </si>
   <si>
-    <t>Solvent</t>
+    <t xml:space="preserve">Solvent application	</t>
+  </si>
+  <si>
+    <t>Solvent application</t>
   </si>
   <si>
     <t>Other</t>
@@ -134,12 +142,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -151,23 +156,14 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -387,359 +383,359 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="34.88"/>
-    <col customWidth="1" min="2" max="3" width="12.63"/>
+    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>2022.0</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>2021.0</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="7" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="8">
+      <c r="A19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="4">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>2011.0</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="4">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="4">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="4">
+      <c r="A25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="4">
+      <c r="A26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="4">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>2011.0</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="12"/>
+      <c r="A28" s="8"/>
     </row>
     <row r="29" ht="15.75" customHeight="1"/>
     <row r="30" ht="15.75" customHeight="1"/>
@@ -1713,14 +1709,6 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
-    <row r="1005" ht="15.75" customHeight="1"/>
-    <row r="1006" ht="15.75" customHeight="1"/>
-    <row r="1007" ht="15.75" customHeight="1"/>
-    <row r="1008" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated usages order for 2019-2021
</commit_message>
<xml_diff>
--- a/core/import_data/resources/usages_cp_format.xlsx
+++ b/core/import_data/resources/usages_cp_format.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="9wLjhp4Lzfao7HxhyYB+SVyU+CvlC69aF0P8vAzjULE="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="7A2mQ5TldcVw2YAxUa7Tfdc8heZILVE4IClT2TaliYI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>usage</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>sections</t>
+  </si>
+  <si>
+    <t>sort_order</t>
   </si>
   <si>
     <t>Aerosol</t>
@@ -123,14 +126,14 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -153,41 +156,40 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -421,385 +423,506 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6">
+        <v>10.0</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1995.0</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
+      <c r="E3" s="6">
+        <v>20.0</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6">
+        <v>30.0</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
-        <v>5</v>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="6">
+        <v>40.0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5" t="s">
-        <v>5</v>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6">
+        <v>50.0</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>1999.0</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>5</v>
+      <c r="D7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6">
+        <v>60.0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="6">
+        <v>10.0</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="6">
+        <v>20.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5" t="s">
-        <v>11</v>
+      <c r="C10" s="5"/>
+      <c r="D10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6">
+        <v>30.0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5" t="s">
-        <v>11</v>
+      <c r="C11" s="5"/>
+      <c r="D11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6">
+        <v>40.0</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5" t="s">
-        <v>11</v>
+      <c r="C12" s="5"/>
+      <c r="D12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="6">
+        <v>50.0</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2022.0</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
-        <v>2022.0</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5" t="s">
-        <v>11</v>
+      <c r="E13" s="6">
+        <v>60.0</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="8">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
-        <v>11</v>
+      <c r="C14" s="9">
+        <v>2021.0</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6">
+        <v>80.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="9">
+        <v>2021.0</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="6">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="8">
-        <v>2019.0</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B16" s="10">
         <v>2021.0</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>11</v>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="6">
+        <v>70.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="10">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="6">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C18" s="4"/>
+      <c r="B18" s="4">
+        <v>2019.0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2021.0</v>
+      </c>
       <c r="D18" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="E18" s="6">
+        <v>90.0</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="8">
-        <v>2019.0</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1995.0</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="6">
+        <v>70.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="8">
-        <v>2019.0</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5" t="s">
-        <v>11</v>
+      <c r="B20" s="4">
+        <v>1995.0</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="6">
+        <v>80.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2019.0</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="6">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B22" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="6">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C23" s="7">
-        <v>2004.0</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>5</v>
+      <c r="B23" s="4">
+        <v>2019.0</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="6">
+        <v>110.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="8">
-        <v>2000.0</v>
-      </c>
-      <c r="C24" s="8">
-        <v>2011.0</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1995.0</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="6">
+        <v>90.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="8">
-        <v>2000.0</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1995.0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>2004.0</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="6">
+        <v>100.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="4">
+        <v>2000.0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2011.0</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="6">
+        <v>110.0</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B27" s="4">
         <v>2000.0</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="5" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="6">
+        <v>120.0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B28" s="4">
+        <v>2000.0</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="6">
+        <v>130.0</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="4">
         <v>1998.0</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="3">
+      <c r="C29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="6">
+        <v>140.0</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4">
         <v>1998.0</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="3">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="6">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C31" s="4">
         <v>2011.0</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="11">
+      <c r="D31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="6">
+        <v>160.0</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="12">
         <v>2000.0</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C32" s="12">
         <v>2001.0</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+      <c r="D32" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="6">
+        <v>170.0</v>
+      </c>
+    </row>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Updated usages order for 2019-2021 (#158)
</commit_message>
<xml_diff>
--- a/core/import_data/resources/usages_cp_format.xlsx
+++ b/core/import_data/resources/usages_cp_format.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="9wLjhp4Lzfao7HxhyYB+SVyU+CvlC69aF0P8vAzjULE="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="7A2mQ5TldcVw2YAxUa7Tfdc8heZILVE4IClT2TaliYI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>usage</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>sections</t>
+  </si>
+  <si>
+    <t>sort_order</t>
   </si>
   <si>
     <t>Aerosol</t>
@@ -123,14 +126,14 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -153,41 +156,40 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -421,385 +423,506 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6">
+        <v>10.0</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1995.0</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
+      <c r="E3" s="6">
+        <v>20.0</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6">
+        <v>30.0</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
-        <v>5</v>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="6">
+        <v>40.0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5" t="s">
-        <v>5</v>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6">
+        <v>50.0</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>1999.0</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>5</v>
+      <c r="D7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6">
+        <v>60.0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="6">
+        <v>10.0</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="6">
+        <v>20.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5" t="s">
-        <v>11</v>
+      <c r="C10" s="5"/>
+      <c r="D10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6">
+        <v>30.0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5" t="s">
-        <v>11</v>
+      <c r="C11" s="5"/>
+      <c r="D11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6">
+        <v>40.0</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5" t="s">
-        <v>11</v>
+      <c r="C12" s="5"/>
+      <c r="D12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="6">
+        <v>50.0</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2022.0</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
-        <v>2022.0</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5" t="s">
-        <v>11</v>
+      <c r="E13" s="6">
+        <v>60.0</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="8">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
-        <v>11</v>
+      <c r="C14" s="9">
+        <v>2021.0</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6">
+        <v>80.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="9">
+        <v>2021.0</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="6">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="8">
-        <v>2019.0</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B16" s="10">
         <v>2021.0</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>11</v>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="6">
+        <v>70.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="10">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="6">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C18" s="4"/>
+      <c r="B18" s="4">
+        <v>2019.0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2021.0</v>
+      </c>
       <c r="D18" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="E18" s="6">
+        <v>90.0</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="8">
-        <v>2019.0</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1995.0</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="6">
+        <v>70.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="8">
-        <v>2019.0</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5" t="s">
-        <v>11</v>
+      <c r="B20" s="4">
+        <v>1995.0</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="6">
+        <v>80.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2019.0</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="6">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B22" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="6">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C23" s="7">
-        <v>2004.0</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>5</v>
+      <c r="B23" s="4">
+        <v>2019.0</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="6">
+        <v>110.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="8">
-        <v>2000.0</v>
-      </c>
-      <c r="C24" s="8">
-        <v>2011.0</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1995.0</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="6">
+        <v>90.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="8">
-        <v>2000.0</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1995.0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>2004.0</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="6">
+        <v>100.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="4">
+        <v>2000.0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2011.0</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="6">
+        <v>110.0</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B27" s="4">
         <v>2000.0</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="5" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="6">
+        <v>120.0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B28" s="4">
+        <v>2000.0</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="6">
+        <v>130.0</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="4">
         <v>1998.0</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="3">
+      <c r="C29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="6">
+        <v>140.0</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4">
         <v>1998.0</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="3">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="6">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C31" s="4">
         <v>2011.0</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="11">
+      <c r="D31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="6">
+        <v>160.0</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="12">
         <v>2000.0</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C32" s="12">
         <v>2001.0</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+      <c r="D32" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="6">
+        <v>170.0</v>
+      </c>
+    </row>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added header name for cp format column
</commit_message>
<xml_diff>
--- a/core/import_data/resources/usages_cp_format.xlsx
+++ b/core/import_data/resources/usages_cp_format.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="7A2mQ5TldcVw2YAxUa7Tfdc8heZILVE4IClT2TaliYI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="z0EuTEAI4w/WDx+tWmVHVzbAJMhe2CJBZsd5t9ITr+Q="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>usage</t>
   </si>
@@ -33,6 +33,9 @@
     <t>sort_order</t>
   </si>
   <si>
+    <t>header_name</t>
+  </si>
+  <si>
     <t>Aerosol</t>
   </si>
   <si>
@@ -57,10 +60,16 @@
     <t>B</t>
   </si>
   <si>
+    <t xml:space="preserve">Refrigeration and air-conditioning </t>
+  </si>
+  <si>
     <t>Refrigeration Manufacturing Refrigeration</t>
   </si>
   <si>
     <t>Refrigeration Manufacturing Other</t>
+  </si>
+  <si>
+    <t>Other unidentified manufacturing</t>
   </si>
   <si>
     <t>Refrigeration Manufacturing Total</t>
@@ -163,33 +172,33 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -407,7 +416,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="34.88"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
+    <col customWidth="1" min="2" max="5" width="12.63"/>
+    <col customWidth="1" min="6" max="6" width="26.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -426,32 +436,34 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4">
         <v>1995.0</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="6">
         <v>10.0</v>
@@ -459,14 +471,14 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>1995.0</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="6">
         <v>20.0</v>
@@ -474,14 +486,14 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4">
         <v>1995.0</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" s="6">
         <v>30.0</v>
@@ -489,14 +501,14 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4">
         <v>1995.0</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="6">
         <v>40.0</v>
@@ -504,14 +516,14 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4">
         <v>1995.0</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="6">
         <v>50.0</v>
@@ -519,7 +531,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4">
         <v>1995.0</v>
@@ -528,7 +540,7 @@
         <v>1999.0</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="6">
         <v>60.0</v>
@@ -536,14 +548,14 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4">
         <v>2019.0</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="6">
         <v>10.0</v>
@@ -551,14 +563,14 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>2019.0</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="6">
         <v>20.0</v>
@@ -566,14 +578,14 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>2019.0</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="6">
         <v>30.0</v>
@@ -581,17 +593,20 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4">
-        <v>2019.0</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2022.0</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="6">
         <v>40.0</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -601,73 +616,75 @@
       <c r="B12" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="10">
+        <v>2021.0</v>
+      </c>
       <c r="D12" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" s="6">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="8" t="s">
-        <v>13</v>
+      <c r="A13" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B13" s="4">
-        <v>2022.0</v>
+        <v>2019.0</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="6">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="6">
         <v>60.0</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4">
-        <v>2019.0</v>
-      </c>
-      <c r="C14" s="9">
-        <v>2021.0</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="6">
-        <v>80.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="5">
         <v>2021.0</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" s="6">
-        <v>70.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="10">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4">
+        <v>2019.0</v>
+      </c>
+      <c r="C16" s="5">
         <v>2021.0</v>
       </c>
-      <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="6">
         <v>70.0</v>
@@ -675,255 +692,272 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="10">
-        <v>2021.0</v>
+        <v>12</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2022.0</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" s="6">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8">
+        <v>2022.0</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="6">
         <v>80.0</v>
       </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="F18" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C19" s="4">
         <v>2021.0</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="D19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="6">
         <v>90.0</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4">
-        <v>1995.0</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="6">
-        <v>70.0</v>
-      </c>
-    </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>17</v>
+      <c r="A20" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B20" s="4">
         <v>1995.0</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E20" s="6">
-        <v>80.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>16</v>
+      <c r="A21" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="B21" s="4">
-        <v>2019.0</v>
+        <v>1995.0</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E21" s="6">
-        <v>100.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>18</v>
+      <c r="A22" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B22" s="4">
         <v>2019.0</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22" s="6">
-        <v>90.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>19</v>
+      <c r="A23" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>2019.0</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>12</v>
+      <c r="D23" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="E23" s="6">
-        <v>110.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
-        <v>1995.0</v>
+        <v>2019.0</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E24" s="6">
-        <v>90.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C25" s="5">
-        <v>2004.0</v>
-      </c>
+      <c r="C25" s="5"/>
       <c r="D25" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E25" s="6">
-        <v>100.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26" s="4">
-        <v>2000.0</v>
-      </c>
-      <c r="C26" s="4">
-        <v>2011.0</v>
+        <v>1995.0</v>
+      </c>
+      <c r="C26" s="5">
+        <v>2004.0</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E26" s="6">
-        <v>110.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B27" s="4">
         <v>2000.0</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="4">
+        <v>2011.0</v>
+      </c>
       <c r="D27" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E27" s="6">
-        <v>120.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" s="4">
         <v>2000.0</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E28" s="6">
-        <v>130.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="7" t="s">
-        <v>25</v>
+      <c r="A29" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B29" s="4">
-        <v>1998.0</v>
+        <v>2000.0</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E29" s="6">
-        <v>140.0</v>
+        <v>130.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30" s="4">
         <v>1998.0</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E30" s="6">
+        <v>140.0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1998.0</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="6">
         <v>150.0</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="4">
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C32" s="4">
         <v>2011.0</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="6">
+      <c r="D32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="6">
         <v>160.0</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="12">
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="6">
         <v>2000.0</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C33" s="6">
         <v>2001.0</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="6">
+      <c r="D33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="6">
         <v>170.0</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
@@ -1892,7 +1926,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added header name for cp format column (#163)
</commit_message>
<xml_diff>
--- a/core/import_data/resources/usages_cp_format.xlsx
+++ b/core/import_data/resources/usages_cp_format.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="7A2mQ5TldcVw2YAxUa7Tfdc8heZILVE4IClT2TaliYI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="z0EuTEAI4w/WDx+tWmVHVzbAJMhe2CJBZsd5t9ITr+Q="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>usage</t>
   </si>
@@ -33,6 +33,9 @@
     <t>sort_order</t>
   </si>
   <si>
+    <t>header_name</t>
+  </si>
+  <si>
     <t>Aerosol</t>
   </si>
   <si>
@@ -57,10 +60,16 @@
     <t>B</t>
   </si>
   <si>
+    <t xml:space="preserve">Refrigeration and air-conditioning </t>
+  </si>
+  <si>
     <t>Refrigeration Manufacturing Refrigeration</t>
   </si>
   <si>
     <t>Refrigeration Manufacturing Other</t>
+  </si>
+  <si>
+    <t>Other unidentified manufacturing</t>
   </si>
   <si>
     <t>Refrigeration Manufacturing Total</t>
@@ -163,33 +172,33 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -407,7 +416,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="34.88"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
+    <col customWidth="1" min="2" max="5" width="12.63"/>
+    <col customWidth="1" min="6" max="6" width="26.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -426,32 +436,34 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4">
         <v>1995.0</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="6">
         <v>10.0</v>
@@ -459,14 +471,14 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>1995.0</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="6">
         <v>20.0</v>
@@ -474,14 +486,14 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4">
         <v>1995.0</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" s="6">
         <v>30.0</v>
@@ -489,14 +501,14 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4">
         <v>1995.0</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="6">
         <v>40.0</v>
@@ -504,14 +516,14 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4">
         <v>1995.0</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="6">
         <v>50.0</v>
@@ -519,7 +531,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4">
         <v>1995.0</v>
@@ -528,7 +540,7 @@
         <v>1999.0</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="6">
         <v>60.0</v>
@@ -536,14 +548,14 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4">
         <v>2019.0</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="6">
         <v>10.0</v>
@@ -551,14 +563,14 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>2019.0</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="6">
         <v>20.0</v>
@@ -566,14 +578,14 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>2019.0</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="6">
         <v>30.0</v>
@@ -581,17 +593,20 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4">
-        <v>2019.0</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2022.0</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="6">
         <v>40.0</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -601,73 +616,75 @@
       <c r="B12" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="10">
+        <v>2021.0</v>
+      </c>
       <c r="D12" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" s="6">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="8" t="s">
-        <v>13</v>
+      <c r="A13" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B13" s="4">
-        <v>2022.0</v>
+        <v>2019.0</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="6">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="6">
         <v>60.0</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4">
-        <v>2019.0</v>
-      </c>
-      <c r="C14" s="9">
-        <v>2021.0</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="6">
-        <v>80.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="5">
         <v>2021.0</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" s="6">
-        <v>70.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="10">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4">
+        <v>2019.0</v>
+      </c>
+      <c r="C16" s="5">
         <v>2021.0</v>
       </c>
-      <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="6">
         <v>70.0</v>
@@ -675,255 +692,272 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="10">
-        <v>2021.0</v>
+        <v>12</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2022.0</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" s="6">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8">
+        <v>2022.0</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="6">
         <v>80.0</v>
       </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="F18" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
         <v>2019.0</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C19" s="4">
         <v>2021.0</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="D19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="6">
         <v>90.0</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4">
-        <v>1995.0</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="6">
-        <v>70.0</v>
-      </c>
-    </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>17</v>
+      <c r="A20" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B20" s="4">
         <v>1995.0</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E20" s="6">
-        <v>80.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>16</v>
+      <c r="A21" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="B21" s="4">
-        <v>2019.0</v>
+        <v>1995.0</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E21" s="6">
-        <v>100.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>18</v>
+      <c r="A22" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B22" s="4">
         <v>2019.0</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22" s="6">
-        <v>90.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>19</v>
+      <c r="A23" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>2019.0</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>12</v>
+      <c r="D23" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="E23" s="6">
-        <v>110.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
-        <v>1995.0</v>
+        <v>2019.0</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E24" s="6">
-        <v>90.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C25" s="5">
-        <v>2004.0</v>
-      </c>
+      <c r="C25" s="5"/>
       <c r="D25" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E25" s="6">
-        <v>100.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26" s="4">
-        <v>2000.0</v>
-      </c>
-      <c r="C26" s="4">
-        <v>2011.0</v>
+        <v>1995.0</v>
+      </c>
+      <c r="C26" s="5">
+        <v>2004.0</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E26" s="6">
-        <v>110.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B27" s="4">
         <v>2000.0</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="4">
+        <v>2011.0</v>
+      </c>
       <c r="D27" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E27" s="6">
-        <v>120.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" s="4">
         <v>2000.0</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E28" s="6">
-        <v>130.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="7" t="s">
-        <v>25</v>
+      <c r="A29" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B29" s="4">
-        <v>1998.0</v>
+        <v>2000.0</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E29" s="6">
-        <v>140.0</v>
+        <v>130.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30" s="4">
         <v>1998.0</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E30" s="6">
+        <v>140.0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1998.0</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="6">
         <v>150.0</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="4">
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="4">
         <v>1995.0</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C32" s="4">
         <v>2011.0</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="6">
+      <c r="D32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="6">
         <v>160.0</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="12">
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="6">
         <v>2000.0</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C33" s="6">
         <v>2001.0</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="6">
+      <c r="D33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="6">
         <v>170.0</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
@@ -1892,7 +1926,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated time frames (2019-2021 -> 2019-2022)
</commit_message>
<xml_diff>
--- a/core/import_data/resources/usages_cp_format.xlsx
+++ b/core/import_data/resources/usages_cp_format.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="z0EuTEAI4w/WDx+tWmVHVzbAJMhe2CJBZsd5t9ITr+Q="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="FgAALCgghD+V0Lm3dIZQxChdBeThnkzcYSlwWNDoehQ="/>
     </ext>
   </extLst>
 </workbook>
@@ -118,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -133,11 +133,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -165,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -173,9 +168,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -189,16 +181,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -436,7 +425,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2"/>
@@ -458,14 +447,14 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>10.0</v>
       </c>
     </row>
@@ -473,14 +462,14 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>20.0</v>
       </c>
     </row>
@@ -488,14 +477,14 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>30.0</v>
       </c>
     </row>
@@ -503,14 +492,14 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>40.0</v>
       </c>
     </row>
@@ -518,14 +507,14 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>50.0</v>
       </c>
     </row>
@@ -533,16 +522,16 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1999.0</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>60.0</v>
       </c>
     </row>
@@ -550,14 +539,14 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>10.0</v>
       </c>
     </row>
@@ -565,14 +554,14 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>20.0</v>
       </c>
     </row>
@@ -580,14 +569,14 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>30.0</v>
       </c>
     </row>
@@ -595,17 +584,17 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
-        <v>2022.0</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7" t="s">
+      <c r="B11" s="7">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>40.0</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -613,16 +602,16 @@
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C12" s="10">
-        <v>2021.0</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="8">
+        <v>2022.0</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>40.0</v>
       </c>
     </row>
@@ -630,29 +619,29 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>50.0</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4">
-        <v>2022.0</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="7" t="s">
+      <c r="B14" s="7">
+        <v>2023.0</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>60.0</v>
       </c>
     </row>
@@ -660,16 +649,16 @@
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C15" s="5">
-        <v>2021.0</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C15" s="8">
+        <v>2022.0</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>80.0</v>
       </c>
     </row>
@@ -677,16 +666,16 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C16" s="5">
-        <v>2021.0</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="8">
+        <v>2022.0</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>70.0</v>
       </c>
     </row>
@@ -694,14 +683,14 @@
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="8">
-        <v>2022.0</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5" t="s">
+      <c r="B17" s="7">
+        <v>2023.0</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>70.0</v>
       </c>
     </row>
@@ -709,34 +698,34 @@
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
+        <v>2023.0</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2019.0</v>
+      </c>
+      <c r="C19" s="7">
         <v>2022.0</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="6">
-        <v>80.0</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4">
-        <v>2019.0</v>
-      </c>
-      <c r="C19" s="4">
-        <v>2021.0</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>90.0</v>
       </c>
     </row>
@@ -744,29 +733,29 @@
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="7" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>70.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="7" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>80.0</v>
       </c>
     </row>
@@ -774,29 +763,29 @@
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>100.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="7" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>90.0</v>
       </c>
     </row>
@@ -804,14 +793,14 @@
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>110.0</v>
       </c>
     </row>
@@ -819,14 +808,14 @@
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>90.0</v>
       </c>
     </row>
@@ -834,16 +823,16 @@
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>2004.0</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>100.0</v>
       </c>
     </row>
@@ -851,16 +840,16 @@
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>2011.0</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>110.0</v>
       </c>
     </row>
@@ -868,14 +857,14 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>120.0</v>
       </c>
     </row>
@@ -883,44 +872,44 @@
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>130.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>1998.0</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>140.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>1998.0</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>150.0</v>
       </c>
     </row>
@@ -928,33 +917,33 @@
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>2011.0</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>160.0</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <v>2000.0</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>2001.0</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <v>170.0</v>
       </c>
     </row>
@@ -1925,7 +1914,6 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated time frames (2019-2021 -> 2019-2022) (#168)
</commit_message>
<xml_diff>
--- a/core/import_data/resources/usages_cp_format.xlsx
+++ b/core/import_data/resources/usages_cp_format.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="z0EuTEAI4w/WDx+tWmVHVzbAJMhe2CJBZsd5t9ITr+Q="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="FgAALCgghD+V0Lm3dIZQxChdBeThnkzcYSlwWNDoehQ="/>
     </ext>
   </extLst>
 </workbook>
@@ -118,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -133,11 +133,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -165,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -173,9 +168,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -189,16 +181,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -436,7 +425,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2"/>
@@ -458,14 +447,14 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>10.0</v>
       </c>
     </row>
@@ -473,14 +462,14 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>20.0</v>
       </c>
     </row>
@@ -488,14 +477,14 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>30.0</v>
       </c>
     </row>
@@ -503,14 +492,14 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>40.0</v>
       </c>
     </row>
@@ -518,14 +507,14 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>50.0</v>
       </c>
     </row>
@@ -533,16 +522,16 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1999.0</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>60.0</v>
       </c>
     </row>
@@ -550,14 +539,14 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>10.0</v>
       </c>
     </row>
@@ -565,14 +554,14 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>20.0</v>
       </c>
     </row>
@@ -580,14 +569,14 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>30.0</v>
       </c>
     </row>
@@ -595,17 +584,17 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
-        <v>2022.0</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7" t="s">
+      <c r="B11" s="7">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>40.0</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -613,16 +602,16 @@
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C12" s="10">
-        <v>2021.0</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="8">
+        <v>2022.0</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>40.0</v>
       </c>
     </row>
@@ -630,29 +619,29 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>50.0</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4">
-        <v>2022.0</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="7" t="s">
+      <c r="B14" s="7">
+        <v>2023.0</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>60.0</v>
       </c>
     </row>
@@ -660,16 +649,16 @@
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C15" s="5">
-        <v>2021.0</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C15" s="8">
+        <v>2022.0</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>80.0</v>
       </c>
     </row>
@@ -677,16 +666,16 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C16" s="5">
-        <v>2021.0</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="8">
+        <v>2022.0</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>70.0</v>
       </c>
     </row>
@@ -694,14 +683,14 @@
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="8">
-        <v>2022.0</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5" t="s">
+      <c r="B17" s="7">
+        <v>2023.0</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>70.0</v>
       </c>
     </row>
@@ -709,34 +698,34 @@
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
+        <v>2023.0</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2019.0</v>
+      </c>
+      <c r="C19" s="7">
         <v>2022.0</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="6">
-        <v>80.0</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4">
-        <v>2019.0</v>
-      </c>
-      <c r="C19" s="4">
-        <v>2021.0</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>90.0</v>
       </c>
     </row>
@@ -744,29 +733,29 @@
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="7" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>70.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="7" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>80.0</v>
       </c>
     </row>
@@ -774,29 +763,29 @@
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>100.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="7" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>90.0</v>
       </c>
     </row>
@@ -804,14 +793,14 @@
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>110.0</v>
       </c>
     </row>
@@ -819,14 +808,14 @@
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>90.0</v>
       </c>
     </row>
@@ -834,16 +823,16 @@
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>2004.0</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>100.0</v>
       </c>
     </row>
@@ -851,16 +840,16 @@
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>2011.0</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>110.0</v>
       </c>
     </row>
@@ -868,14 +857,14 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>120.0</v>
       </c>
     </row>
@@ -883,44 +872,44 @@
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>130.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>1998.0</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>140.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>1998.0</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>150.0</v>
       </c>
     </row>
@@ -928,33 +917,33 @@
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>2011.0</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>160.0</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <v>2000.0</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>2001.0</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <v>170.0</v>
       </c>
     </row>
@@ -1925,7 +1914,6 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Udpated imports + fix sort blends bug (get records)
</commit_message>
<xml_diff>
--- a/core/import_data/resources/usages_cp_format.xlsx
+++ b/core/import_data/resources/usages_cp_format.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="FgAALCgghD+V0Lm3dIZQxChdBeThnkzcYSlwWNDoehQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="KRFAggEkqqTG/2KQyIKMiqJBMbr1Rd/DG9DRX2V9oxU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="33">
   <si>
     <t>usage</t>
   </si>
@@ -54,6 +54,9 @@
     <t>Refrigeration Manufacturing</t>
   </si>
   <si>
+    <t>Refrigeration Servicing</t>
+  </si>
+  <si>
     <t>Refrigeration Manufacturing AC</t>
   </si>
   <si>
@@ -75,10 +78,10 @@
     <t>Refrigeration Manufacturing Total</t>
   </si>
   <si>
-    <t>Refrigeration Servicing</t>
-  </si>
-  <si>
     <t xml:space="preserve">Solvent application	</t>
+  </si>
+  <si>
+    <t>Solvent</t>
   </si>
   <si>
     <t>Solvent application</t>
@@ -118,7 +121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -138,6 +141,11 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -160,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -179,13 +187,22 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -510,446 +527,509 @@
       <c r="B6" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="7">
+        <v>2004.0</v>
+      </c>
       <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="5">
         <v>50.0</v>
       </c>
+      <c r="F6" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1999.0</v>
-      </c>
-      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2005.0</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="5">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="5">
-        <v>10.0</v>
+        <v>1995.0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2004.0</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="10">
+        <v>60.0</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>1995.0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1999.0</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="5">
-        <v>20.0</v>
+        <v>7</v>
+      </c>
+      <c r="E9" s="10">
+        <v>70.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3">
         <v>2019.0</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="6" t="s">
-        <v>13</v>
+      <c r="D10" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E10" s="5">
-        <v>30.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7">
-        <v>2023.0</v>
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2019.0</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="6" t="s">
-        <v>13</v>
+      <c r="D11" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E11" s="5">
-        <v>40.0</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>14</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C12" s="8">
-        <v>2022.0</v>
-      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E12" s="5">
-        <v>40.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
-        <v>2019.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="5">
-        <v>50.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="7">
-        <v>2023.0</v>
-      </c>
-      <c r="C14" s="4"/>
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2019.0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2022.0</v>
+      </c>
       <c r="D14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" s="5">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C15" s="8">
-        <v>2022.0</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>13</v>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E15" s="5">
-        <v>80.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C16" s="8">
-        <v>2022.0</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>13</v>
+        <v>2023.0</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E16" s="5">
-        <v>70.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="7">
-        <v>2023.0</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2019.0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2022.0</v>
+      </c>
       <c r="D17" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17" s="5">
-        <v>70.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2019.0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2022.0</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="5">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="3">
         <v>2023.0</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="5">
-        <v>80.0</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2022.0</v>
-      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19" s="5">
-        <v>90.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2023.0</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="5">
-        <v>70.0</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="B21" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="6" t="s">
-        <v>7</v>
+        <v>2019.0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2022.0</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E21" s="5">
-        <v>80.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="3">
-        <v>2019.0</v>
+        <v>12</v>
+      </c>
+      <c r="B22" s="9">
+        <v>2005.0</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E22" s="5">
-        <v>100.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1995.0</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>21</v>
-      </c>
-      <c r="B23" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="5">
-        <v>90.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B24" s="3">
         <v>2019.0</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
-        <v>13</v>
+      <c r="D24" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E24" s="5">
-        <v>110.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3">
-        <v>1995.0</v>
+        <v>2019.0</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
-        <v>7</v>
+      <c r="D25" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E25" s="5">
         <v>90.0</v>
       </c>
+      <c r="F25" s="12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C26" s="4">
-        <v>2004.0</v>
-      </c>
+        <v>2019.0</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E26" s="5">
-        <v>100.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="3">
-        <v>2000.0</v>
-      </c>
-      <c r="C27" s="3">
-        <v>2011.0</v>
-      </c>
+        <v>1995.0</v>
+      </c>
+      <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="5">
-        <v>110.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="3">
-        <v>2000.0</v>
-      </c>
-      <c r="C28" s="4"/>
+        <v>1995.0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>2004.0</v>
+      </c>
       <c r="D28" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="5">
-        <v>120.0</v>
+        <v>100.0</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="3">
+        <v>2011.0</v>
+      </c>
       <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="5">
-        <v>130.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>28</v>
+      <c r="A30" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B30" s="3">
-        <v>1998.0</v>
+        <v>2000.0</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="5">
-        <v>140.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="6" t="s">
-        <v>29</v>
+      <c r="A31" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B31" s="3">
-        <v>1998.0</v>
+        <v>2000.0</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="5">
-        <v>150.0</v>
+        <v>130.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="1" t="s">
-        <v>30</v>
+      <c r="A32" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B32" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C32" s="3">
-        <v>2011.0</v>
-      </c>
+        <v>1998.0</v>
+      </c>
+      <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="5">
+        <v>140.0</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1998.0</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="5">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1995.0</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2011.0</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="5">
         <v>160.0</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="5">
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="5">
         <v>2000.0</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C35" s="5">
         <v>2001.0</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E35" s="5">
         <v>170.0</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="12">
+        <v>1995.0</v>
+      </c>
+      <c r="C36" s="12">
+        <v>2004.0</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="12">
+        <v>280.0</v>
+      </c>
+    </row>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
@@ -1914,6 +1994,8 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Udpated imports + fix sort blends bug (get records) (#211)
</commit_message>
<xml_diff>
--- a/core/import_data/resources/usages_cp_format.xlsx
+++ b/core/import_data/resources/usages_cp_format.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="FgAALCgghD+V0Lm3dIZQxChdBeThnkzcYSlwWNDoehQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="KRFAggEkqqTG/2KQyIKMiqJBMbr1Rd/DG9DRX2V9oxU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="33">
   <si>
     <t>usage</t>
   </si>
@@ -54,6 +54,9 @@
     <t>Refrigeration Manufacturing</t>
   </si>
   <si>
+    <t>Refrigeration Servicing</t>
+  </si>
+  <si>
     <t>Refrigeration Manufacturing AC</t>
   </si>
   <si>
@@ -75,10 +78,10 @@
     <t>Refrigeration Manufacturing Total</t>
   </si>
   <si>
-    <t>Refrigeration Servicing</t>
-  </si>
-  <si>
     <t xml:space="preserve">Solvent application	</t>
+  </si>
+  <si>
+    <t>Solvent</t>
   </si>
   <si>
     <t>Solvent application</t>
@@ -118,7 +121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -138,6 +141,11 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -160,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -179,13 +187,22 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -510,446 +527,509 @@
       <c r="B6" s="3">
         <v>1995.0</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="7">
+        <v>2004.0</v>
+      </c>
       <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="5">
         <v>50.0</v>
       </c>
+      <c r="F6" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1999.0</v>
-      </c>
-      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2005.0</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="5">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="5">
-        <v>10.0</v>
+        <v>1995.0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2004.0</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="10">
+        <v>60.0</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>1995.0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1999.0</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="5">
-        <v>20.0</v>
+        <v>7</v>
+      </c>
+      <c r="E9" s="10">
+        <v>70.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3">
         <v>2019.0</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="6" t="s">
-        <v>13</v>
+      <c r="D10" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E10" s="5">
-        <v>30.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7">
-        <v>2023.0</v>
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2019.0</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="6" t="s">
-        <v>13</v>
+      <c r="D11" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E11" s="5">
-        <v>40.0</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>14</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C12" s="8">
-        <v>2022.0</v>
-      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E12" s="5">
-        <v>40.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
-        <v>2019.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="5">
-        <v>50.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="7">
-        <v>2023.0</v>
-      </c>
-      <c r="C14" s="4"/>
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2019.0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2022.0</v>
+      </c>
       <c r="D14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" s="5">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3">
         <v>2019.0</v>
       </c>
-      <c r="C15" s="8">
-        <v>2022.0</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>13</v>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E15" s="5">
-        <v>80.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C16" s="8">
-        <v>2022.0</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>13</v>
+        <v>2023.0</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E16" s="5">
-        <v>70.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="7">
-        <v>2023.0</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2019.0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2022.0</v>
+      </c>
       <c r="D17" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17" s="5">
-        <v>70.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2019.0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2022.0</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="5">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="3">
         <v>2023.0</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="5">
-        <v>80.0</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2022.0</v>
-      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19" s="5">
-        <v>90.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2023.0</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="5">
-        <v>70.0</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="B21" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="6" t="s">
-        <v>7</v>
+        <v>2019.0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2022.0</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E21" s="5">
-        <v>80.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="3">
-        <v>2019.0</v>
+        <v>12</v>
+      </c>
+      <c r="B22" s="9">
+        <v>2005.0</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E22" s="5">
-        <v>100.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1995.0</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>21</v>
-      </c>
-      <c r="B23" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="5">
-        <v>90.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B24" s="3">
         <v>2019.0</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
-        <v>13</v>
+      <c r="D24" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E24" s="5">
-        <v>110.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3">
-        <v>1995.0</v>
+        <v>2019.0</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
-        <v>7</v>
+      <c r="D25" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E25" s="5">
         <v>90.0</v>
       </c>
+      <c r="F25" s="12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C26" s="4">
-        <v>2004.0</v>
-      </c>
+        <v>2019.0</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E26" s="5">
-        <v>100.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="3">
-        <v>2000.0</v>
-      </c>
-      <c r="C27" s="3">
-        <v>2011.0</v>
-      </c>
+        <v>1995.0</v>
+      </c>
+      <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="5">
-        <v>110.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="3">
-        <v>2000.0</v>
-      </c>
-      <c r="C28" s="4"/>
+        <v>1995.0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>2004.0</v>
+      </c>
       <c r="D28" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="5">
-        <v>120.0</v>
+        <v>100.0</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="3">
         <v>2000.0</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="3">
+        <v>2011.0</v>
+      </c>
       <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="5">
-        <v>130.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>28</v>
+      <c r="A30" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B30" s="3">
-        <v>1998.0</v>
+        <v>2000.0</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="5">
-        <v>140.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="6" t="s">
-        <v>29</v>
+      <c r="A31" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B31" s="3">
-        <v>1998.0</v>
+        <v>2000.0</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="5">
-        <v>150.0</v>
+        <v>130.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="1" t="s">
-        <v>30</v>
+      <c r="A32" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B32" s="3">
-        <v>1995.0</v>
-      </c>
-      <c r="C32" s="3">
-        <v>2011.0</v>
-      </c>
+        <v>1998.0</v>
+      </c>
+      <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="5">
+        <v>140.0</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1998.0</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="5">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1995.0</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2011.0</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="5">
         <v>160.0</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="5">
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="5">
         <v>2000.0</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C35" s="5">
         <v>2001.0</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E35" s="5">
         <v>170.0</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="12">
+        <v>1995.0</v>
+      </c>
+      <c r="C36" s="12">
+        <v>2004.0</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="12">
+        <v>280.0</v>
+      </c>
+    </row>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
@@ -1914,6 +1994,8 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>